<commit_message>
finished adding all data to dados_individuos
</commit_message>
<xml_diff>
--- a/dados_individuos.xlsx
+++ b/dados_individuos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gait_patterns_spastic_displegia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvent\Desktop\gait_patterns_spastic_displegia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC807898-2523-414D-8759-5B964752AEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D28DEED-1745-4941-BF0E-03BC2CC8C3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EDB4B48-7705-4D24-93FB-44F7573A8728}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EDB4B48-7705-4D24-93FB-44F7573A8728}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>code</t>
   </si>
@@ -44,12 +44,6 @@
     <t>weight</t>
   </si>
   <si>
-    <t>left_comments</t>
-  </si>
-  <si>
-    <t>right_comments</t>
-  </si>
-  <si>
     <t>CR001</t>
   </si>
   <si>
@@ -75,6 +69,168 @@
   </si>
   <si>
     <t>CR012</t>
+  </si>
+  <si>
+    <t>CR013</t>
+  </si>
+  <si>
+    <t>CR014</t>
+  </si>
+  <si>
+    <t>CR015</t>
+  </si>
+  <si>
+    <t>CR016</t>
+  </si>
+  <si>
+    <t>CR017</t>
+  </si>
+  <si>
+    <t>CR018</t>
+  </si>
+  <si>
+    <t>CR019</t>
+  </si>
+  <si>
+    <t>CR020</t>
+  </si>
+  <si>
+    <t>CR021</t>
+  </si>
+  <si>
+    <t>CR022</t>
+  </si>
+  <si>
+    <t>CR023</t>
+  </si>
+  <si>
+    <t>CR024</t>
+  </si>
+  <si>
+    <t>CR025</t>
+  </si>
+  <si>
+    <t>CR026</t>
+  </si>
+  <si>
+    <t>CR027</t>
+  </si>
+  <si>
+    <t>CR028</t>
+  </si>
+  <si>
+    <t>PC002</t>
+  </si>
+  <si>
+    <t>PC003</t>
+  </si>
+  <si>
+    <t>PC004</t>
+  </si>
+  <si>
+    <t>PC005</t>
+  </si>
+  <si>
+    <t>PC006</t>
+  </si>
+  <si>
+    <t>PC007</t>
+  </si>
+  <si>
+    <t>PC008</t>
+  </si>
+  <si>
+    <t>PC009</t>
+  </si>
+  <si>
+    <t>PC010</t>
+  </si>
+  <si>
+    <t>PC011</t>
+  </si>
+  <si>
+    <t>PC012</t>
+  </si>
+  <si>
+    <t>PC013</t>
+  </si>
+  <si>
+    <t>PC014</t>
+  </si>
+  <si>
+    <t>PC015</t>
+  </si>
+  <si>
+    <t>PC016</t>
+  </si>
+  <si>
+    <t>PC017</t>
+  </si>
+  <si>
+    <t>PC018</t>
+  </si>
+  <si>
+    <t>PC019</t>
+  </si>
+  <si>
+    <t>PC020</t>
+  </si>
+  <si>
+    <t>PC021</t>
+  </si>
+  <si>
+    <t>PC022</t>
+  </si>
+  <si>
+    <t>PC023</t>
+  </si>
+  <si>
+    <t>PC026</t>
+  </si>
+  <si>
+    <t>PC028</t>
+  </si>
+  <si>
+    <t>PC029</t>
+  </si>
+  <si>
+    <t>PC030</t>
+  </si>
+  <si>
+    <t>left_leg_comments</t>
+  </si>
+  <si>
+    <t>right_leg_comments</t>
+  </si>
+  <si>
+    <t>left_leg</t>
+  </si>
+  <si>
+    <t>right_leg</t>
+  </si>
+  <si>
+    <t>Crouch Gait</t>
+  </si>
+  <si>
+    <t>Apparent Equinus</t>
+  </si>
+  <si>
+    <t>Jump Gait</t>
+  </si>
+  <si>
+    <t>True Equinus</t>
+  </si>
+  <si>
+    <t>Mild</t>
+  </si>
+  <si>
+    <t>Borderline</t>
+  </si>
+  <si>
+    <t>Difficult</t>
+  </si>
+  <si>
+    <t>Or mild crouch</t>
   </si>
 </sst>
 </file>
@@ -110,10 +266,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,81 +588,654 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33255090-8A6B-4230-A095-B79B7F8C54EA}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="2">
+        <v>22.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="2">
+        <v>22.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>22.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="2">
+        <v>24.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>22.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2">
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="2">
+        <v>24.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="2">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="2">
+        <v>35.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="2">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="2">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="2">
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>33.85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>28.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>26.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>36.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>25.35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>31.25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>44.75</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>40</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>25.75</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <v>36.1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>21</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2">
+        <v>71.5</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
+        <v>25</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2">
+        <v>48.9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2">
+        <v>44.7</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2">
+        <v>49.5</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2">
+        <v>29.3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="2">
+        <v>45.9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="2">
+        <v>42</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>50.9</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2">
+        <v>46.7</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2">
+        <v>37.1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2">
+        <v>31.3</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="2">
+        <v>32</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2">
+        <v>43</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2">
+        <v>42.4</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="2">
+        <v>60</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>